<commit_message>
Further adjsutment and documentation of platemap functions.
</commit_message>
<xml_diff>
--- a/Validation/generated_platemap.xlsx
+++ b/Validation/generated_platemap.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -47,7 +47,10 @@
     <t xml:space="preserve">dilution_series</t>
   </si>
   <si>
-    <t xml:space="preserve">promega_plate_paths</t>
+    <t xml:space="preserve">promega_plate_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file_creation_date</t>
   </si>
   <si>
     <t xml:space="preserve">example1</t>
@@ -132,14 +135,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,8 +172,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,6 +505,9 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2"/>
@@ -503,14 +517,17 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="3">
@@ -521,14 +538,17 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="4">
@@ -539,14 +559,17 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="5">
@@ -557,14 +580,17 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="6">
@@ -575,14 +601,17 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="7">
@@ -593,14 +622,17 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="8">
@@ -611,14 +643,17 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="9">
@@ -629,14 +664,17 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="10">
@@ -647,14 +685,17 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="11">
@@ -665,14 +706,17 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>44808</v>
       </c>
     </row>
     <row r="12">
@@ -683,14 +727,17 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>45367</v>
       </c>
     </row>
     <row r="13">
@@ -701,14 +748,17 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
       <c r="L13" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>45367</v>
       </c>
     </row>
     <row r="14">
@@ -719,14 +769,17 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
       <c r="L14" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>45367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>